<commit_message>
1. XLS files regenerated to fix enum value: description issue.
</commit_message>
<xml_diff>
--- a/cmip6/models/gfdl-am4/cmip6_noaa-gfdl_gfdl-am4_land.xlsx
+++ b/cmip6/models/gfdl-am4/cmip6_noaa-gfdl_gfdl-am4_land.xlsx
@@ -876,10 +876,10 @@
     <t>cmip6.land.soil.hydrology.lateral_connectivity</t>
   </si>
   <si>
-    <t>Perfect connectivity</t>
-  </si>
-  <si>
-    <t>Darcian flow</t>
+    <t>Perfect connectivity: Common soil for multiple tiles</t>
+  </si>
+  <si>
+    <t>Darcian flow: Darcian flow among hillslope tiles</t>
   </si>
   <si>
     <t>3.4.1.7 *</t>

</xml_diff>